<commit_message>
Added logo, improved search UI, other minor improvements
</commit_message>
<xml_diff>
--- a/Expansions and Symbols with code.xlsx
+++ b/Expansions and Symbols with code.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="331">
   <si>
     <t>Core Sets</t>
   </si>
@@ -1002,6 +1002,12 @@
   </si>
   <si>
     <t>HalfR</t>
+  </si>
+  <si>
+    <t>PPR</t>
+  </si>
+  <si>
+    <t>Promo set for Gatherer</t>
   </si>
 </sst>
 </file>
@@ -1333,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F122"/>
+  <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1350,92 +1356,122 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="C1" t="s">
-        <v>195</v>
+        <v>167</v>
+      </c>
+      <c r="E1" t="s">
+        <v>168</v>
       </c>
       <c r="F1" t="str">
         <f>A1&amp;","&amp;B1&amp;","&amp;C1&amp;","&amp;D1&amp;","&amp;E1</f>
-        <v>Expansions,ARB,Alara Reborn,,</v>
+        <v>Core Sets,10E,Tenth Edition,,10th Edition</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
       </c>
       <c r="F2" t="str">
-        <f t="shared" ref="F2:F65" si="0">A2&amp;","&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2</f>
-        <v>Expansions,AL,Alliances,,</v>
+        <f>A2&amp;","&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2</f>
+        <v>Core Sets,1E,Limited Edition Alpha,A,1st Limited Edition Alpha</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,AQ,Antiquities,,</v>
+        <f>A3&amp;","&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3</f>
+        <v>Core Sets,2E,Limited Edition Beta,B,1st Limited Edition Beta</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,AP,Apocalypse,,</v>
+        <f>A4&amp;","&amp;B4&amp;","&amp;C4&amp;","&amp;D4&amp;","&amp;E4</f>
+        <v>Core Sets,2U,Unlimited Edition,U,2nd Unlimited</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,AN,Arabian Nights,,</v>
+        <f>A5&amp;","&amp;B5&amp;","&amp;C5&amp;","&amp;D5&amp;","&amp;E5</f>
+        <v>Core Sets,3E,Revised Edition,R,3rd Revised Edition</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>218</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>219</v>
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,ARC,Archenemy,,</v>
+        <f>A6&amp;","&amp;B6&amp;","&amp;C6&amp;","&amp;D6&amp;","&amp;E6</f>
+        <v>Core Sets,4E,Fourth Edition,,4th Edition</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1443,131 +1479,143 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>259</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
-        <v>258</v>
+        <v>134</v>
+      </c>
+      <c r="D7" t="s">
+        <v>135</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,AVR,Avacyn Restored,,</v>
+        <f>A7&amp;","&amp;B7&amp;","&amp;C7&amp;","&amp;D7&amp;","&amp;E7</f>
+        <v>Expansions,5DN,Fifth Dawn,FD,</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,BR,Battle Royale Box Set,BRB,Battle Royale</v>
+        <f>A8&amp;","&amp;B8&amp;","&amp;C8&amp;","&amp;D8&amp;","&amp;E8</f>
+        <v>Core Sets,5E,Fifth Edition,,5th Edition</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,BD,Beatdown Box Set,,Beatdown</v>
+        <f>A9&amp;","&amp;B9&amp;","&amp;C9&amp;","&amp;D9&amp;","&amp;E9</f>
+        <v>Core Sets,6E,Classic Sixth Edition,,6th Classic Edition</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
-        <v>141</v>
+        <v>103</v>
+      </c>
+      <c r="E10" t="s">
+        <v>104</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,BOK,Betrayers of Kamigawa,,</v>
+        <f>A10&amp;","&amp;B10&amp;","&amp;C10&amp;","&amp;D10&amp;","&amp;E10</f>
+        <v>Core Sets,7E,Seventh Edition,,7th Edition</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>261</v>
+        <v>123</v>
       </c>
       <c r="C11" t="s">
-        <v>260</v>
+        <v>124</v>
+      </c>
+      <c r="D11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" t="s">
+        <v>126</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,BNG,Born of the Gods,,</v>
+        <f>A11&amp;","&amp;B11&amp;","&amp;C11&amp;","&amp;D11&amp;","&amp;E11</f>
+        <v>Core Sets,8ED,Eighth Edition,8E,8th Edition</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C12" t="s">
-        <v>137</v>
+        <v>145</v>
+      </c>
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" t="s">
+        <v>147</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,CHK,Champions of Kamigawa,,</v>
+        <f>A12&amp;","&amp;B12&amp;","&amp;C12&amp;","&amp;D12&amp;","&amp;E12</f>
+        <v>Core Sets,9ED,Ninth Edition,9E,9th Edition</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,CH,Chronicles,,</v>
+        <f>A13&amp;","&amp;B13&amp;","&amp;C13&amp;","&amp;D13&amp;","&amp;E13</f>
+        <v>Expansions,AL,Alliances,,</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>183</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" t="s">
-        <v>73</v>
+        <v>184</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v>Core Sets,6E,Classic Sixth Edition,,6th Classic Edition</v>
+        <f>A14&amp;","&amp;B14&amp;","&amp;C14&amp;","&amp;D14&amp;","&amp;E14</f>
+        <v>Expansions,ALA,Shards of Alara,,</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1575,80 +1623,74 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D15" t="s">
-        <v>157</v>
+        <v>15</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,CSP,Coldsnap,CS,</v>
+        <f>A15&amp;","&amp;B15&amp;","&amp;C15&amp;","&amp;D15&amp;","&amp;E15</f>
+        <v>Expansions,AN,Arabian Nights,,</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>263</v>
+        <v>105</v>
       </c>
       <c r="C16" t="s">
-        <v>262</v>
+        <v>106</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,CMD,Commander,,</v>
+        <f>A16&amp;","&amp;B16&amp;","&amp;C16&amp;","&amp;D16&amp;","&amp;E16</f>
+        <v>Expansions,AP,Apocalypse,,</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>265</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>264</v>
+        <v>17</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,C13,Commander (2013 Edition),,</v>
+        <f>A17&amp;","&amp;B17&amp;","&amp;C17&amp;","&amp;D17&amp;","&amp;E17</f>
+        <v>Expansions,AQ,Antiquities,,</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>267</v>
+        <v>194</v>
       </c>
       <c r="C18" t="s">
-        <v>266</v>
+        <v>195</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,CM1,Commander's Arsenal,,</v>
+        <f>A18&amp;","&amp;B18&amp;","&amp;C18&amp;","&amp;D18&amp;","&amp;E18</f>
+        <v>Expansions,ARB,Alara Reborn,,</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
       <c r="C19" t="s">
-        <v>189</v>
-      </c>
-      <c r="D19" t="s">
-        <v>190</v>
+        <v>219</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,CON,Conflux,CFX,</v>
+        <f>A19&amp;","&amp;B19&amp;","&amp;C19&amp;","&amp;D19&amp;","&amp;E19</f>
+        <v>Special Sets,ARC,Archenemy,,</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1656,32 +1698,32 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="C20" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,DKA,Dark Ascension,,</v>
+        <f>A20&amp;","&amp;B20&amp;","&amp;C20&amp;","&amp;D20&amp;","&amp;E20</f>
+        <v>Expansions,AVR,Avacyn Restored,,</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>131</v>
-      </c>
-      <c r="D21" t="s">
-        <v>132</v>
+        <v>98</v>
+      </c>
+      <c r="E21" t="s">
+        <v>99</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,DST,Darksteel,DS,</v>
+        <f>A21&amp;","&amp;B21&amp;","&amp;C21&amp;","&amp;D21&amp;","&amp;E21</f>
+        <v>Special Sets,BD,Beatdown Box Set,,Beatdown</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1689,14 +1731,14 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
+        <v>261</v>
       </c>
       <c r="C22" t="s">
-        <v>154</v>
+        <v>260</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,DIS,Dissension,,</v>
+        <f>A22&amp;","&amp;B22&amp;","&amp;C22&amp;","&amp;D22&amp;","&amp;E22</f>
+        <v>Expansions,BNG,Born of the Gods,,</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1704,14 +1746,14 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>269</v>
+        <v>140</v>
       </c>
       <c r="C23" t="s">
-        <v>268</v>
+        <v>141</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,DGM,Dragon's Maze,,</v>
+        <f>A23&amp;","&amp;B23&amp;","&amp;C23&amp;","&amp;D23&amp;","&amp;E23</f>
+        <v>Expansions,BOK,Betrayers of Kamigawa,,</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1719,17 +1761,20 @@
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>245</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>246</v>
+        <v>84</v>
+      </c>
+      <c r="D24" t="s">
+        <v>85</v>
       </c>
       <c r="E24" t="s">
-        <v>247</v>
+        <v>86</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,DDH,Duel Decks: Ajani vs. Nicol Bolas,,Duel Decks - Ajani vs. Nicol Bolas</v>
+        <f>A24&amp;","&amp;B24&amp;","&amp;C24&amp;","&amp;D24&amp;","&amp;E24</f>
+        <v>Special Sets,BR,Battle Royale Box Set,BRB,Battle Royale</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1737,35 +1782,32 @@
         <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>191</v>
+        <v>265</v>
       </c>
       <c r="C25" t="s">
-        <v>192</v>
-      </c>
-      <c r="E25" t="s">
-        <v>193</v>
+        <v>264</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,DDC,Duel Decks: Divine vs. Demonic,,Duel Decks - Divine vs. Demonic</v>
+        <f>A25&amp;","&amp;B25&amp;","&amp;C25&amp;","&amp;D25&amp;","&amp;E25</f>
+        <v>Special Sets,C13,Commander (2013 Edition),,</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>225</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>226</v>
-      </c>
-      <c r="E26" t="s">
-        <v>227</v>
+        <v>75</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,DDF,Duel Decks: Elspeth vs. Tezzeret,,Duel Decks - Elspeth vs. Tezzeret</v>
+        <f>A26&amp;","&amp;B26&amp;","&amp;C26&amp;","&amp;D26&amp;","&amp;E26</f>
+        <v>Expansions,CG,Urza's Destiny,UD,</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1773,35 +1815,29 @@
         <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>171</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>172</v>
-      </c>
-      <c r="E27" t="s">
-        <v>173</v>
+        <v>36</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,EVG,Duel Decks: Elves vs. Goblins,,Duel Decks - Elves vs. Goblins</v>
+        <f>A27&amp;","&amp;B27&amp;","&amp;C27&amp;","&amp;D27&amp;","&amp;E27</f>
+        <v>Special Sets,CH,Chronicles,,</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>205</v>
+        <v>136</v>
       </c>
       <c r="C28" t="s">
-        <v>206</v>
-      </c>
-      <c r="E28" t="s">
-        <v>207</v>
+        <v>137</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,DDD,Duel Decks: Garruk vs. Liliana,,Duel Decks - Garruk vs. Liliana</v>
+        <f>A28&amp;","&amp;B28&amp;","&amp;C28&amp;","&amp;D28&amp;","&amp;E28</f>
+        <v>Expansions,CHK,Champions of Kamigawa,,</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1809,17 +1845,14 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C29" t="s">
-        <v>270</v>
-      </c>
-      <c r="E29" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,DDL,Duel Decks: Heroes vs. Monsters,,Duel Decks: Heroes vs. Monsters</v>
+        <f>A29&amp;","&amp;B29&amp;","&amp;C29&amp;","&amp;D29&amp;","&amp;E29</f>
+        <v>Special Sets,CM1,Commander's Arsenal,,</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1827,53 +1860,50 @@
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="C30" t="s">
-        <v>272</v>
-      </c>
-      <c r="E30" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,DDJ,Duel Decks: Izzet vs. Golgari,,Duel Decks: Izzet vs. Golgari</v>
+        <f>A30&amp;","&amp;B30&amp;","&amp;C30&amp;","&amp;D30&amp;","&amp;E30</f>
+        <v>Special Sets,CMD,Commander,,</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C31" t="s">
-        <v>186</v>
-      </c>
-      <c r="E31" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="D31" t="s">
+        <v>190</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,DD2,Duel Decks: Jace vs. Chandra,,Duel Decks - Jace vs. Chandra</v>
+        <f>A31&amp;","&amp;B31&amp;","&amp;C31&amp;","&amp;D31&amp;","&amp;E31</f>
+        <v>Expansions,CON,Conflux,CFX,</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>235</v>
+        <v>155</v>
       </c>
       <c r="C32" t="s">
-        <v>236</v>
-      </c>
-      <c r="E32" t="s">
-        <v>237</v>
+        <v>156</v>
+      </c>
+      <c r="D32" t="s">
+        <v>157</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,DDG,Duel Decks: Knights vs. Dragons,,Duel Decks - Knights vs. Dragons</v>
+        <f>A32&amp;","&amp;B32&amp;","&amp;C32&amp;","&amp;D32&amp;","&amp;E32</f>
+        <v>Expansions,CSP,Coldsnap,CS,</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1881,17 +1911,17 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
       <c r="C33" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="E33" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,DDE,Duel Decks: Phyrexia vs. the Coalition,,Duel Decks - Phyrexia vs. The Coalition</v>
+        <f>A33&amp;","&amp;B33&amp;","&amp;C33&amp;","&amp;D33&amp;","&amp;E33</f>
+        <v>Special Sets,DD2,Duel Decks: Jace vs. Chandra,,Duel Decks - Jace vs. Chandra</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1899,17 +1929,17 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>275</v>
+        <v>191</v>
       </c>
       <c r="C34" t="s">
-        <v>274</v>
+        <v>192</v>
       </c>
       <c r="E34" t="s">
-        <v>274</v>
+        <v>193</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,DDK,Duel Decks: Sorin vs. Tibalt,,Duel Decks: Sorin vs. Tibalt</v>
+        <f>A34&amp;","&amp;B34&amp;","&amp;C34&amp;","&amp;D34&amp;","&amp;E34</f>
+        <v>Special Sets,DDC,Duel Decks: Divine vs. Demonic,,Duel Decks - Divine vs. Demonic</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1917,137 +1947,143 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>255</v>
+        <v>205</v>
       </c>
       <c r="C35" t="s">
-        <v>256</v>
+        <v>206</v>
       </c>
       <c r="E35" t="s">
-        <v>257</v>
+        <v>207</v>
       </c>
       <c r="F35" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,DDI,Duel Decks: Venser vs. Koth,,Duel Decks - Venser vs. Koth</v>
+        <f>A35&amp;","&amp;B35&amp;","&amp;C35&amp;","&amp;D35&amp;","&amp;E35</f>
+        <v>Special Sets,DDD,Duel Decks: Garruk vs. Liliana,,Duel Decks - Garruk vs. Liliana</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>123</v>
+        <v>213</v>
       </c>
       <c r="C36" t="s">
-        <v>124</v>
-      </c>
-      <c r="D36" t="s">
-        <v>125</v>
+        <v>214</v>
       </c>
       <c r="E36" t="s">
-        <v>126</v>
+        <v>215</v>
       </c>
       <c r="F36" t="str">
-        <f t="shared" si="0"/>
-        <v>Core Sets,8ED,Eighth Edition,8E,8th Edition</v>
+        <f>A36&amp;","&amp;B36&amp;","&amp;C36&amp;","&amp;D36&amp;","&amp;E36</f>
+        <v>Special Sets,DDE,Duel Decks: Phyrexia vs. the Coalition,,Duel Decks - Phyrexia vs. The Coalition</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>178</v>
+        <v>225</v>
       </c>
       <c r="C37" t="s">
-        <v>179</v>
+        <v>226</v>
+      </c>
+      <c r="E37" t="s">
+        <v>227</v>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,EVE,Eventide,,</v>
+        <f>A37&amp;","&amp;B37&amp;","&amp;C37&amp;","&amp;D37&amp;","&amp;E37</f>
+        <v>Special Sets,DDF,Duel Decks: Elspeth vs. Tezzeret,,Duel Decks - Elspeth vs. Tezzeret</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>235</v>
       </c>
       <c r="C38" t="s">
-        <v>60</v>
+        <v>236</v>
+      </c>
+      <c r="E38" t="s">
+        <v>237</v>
       </c>
       <c r="F38" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,EX,Exodus,,</v>
+        <f>A38&amp;","&amp;B38&amp;","&amp;C38&amp;","&amp;D38&amp;","&amp;E38</f>
+        <v>Special Sets,DDG,Duel Decks: Knights vs. Dragons,,Duel Decks - Knights vs. Dragons</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>245</v>
       </c>
       <c r="C39" t="s">
-        <v>28</v>
+        <v>246</v>
+      </c>
+      <c r="E39" t="s">
+        <v>247</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,FE,Fallen Empires,,</v>
+        <f>A39&amp;","&amp;B39&amp;","&amp;C39&amp;","&amp;D39&amp;","&amp;E39</f>
+        <v>Special Sets,DDH,Duel Decks: Ajani vs. Nicol Bolas,,Duel Decks - Ajani vs. Nicol Bolas</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>133</v>
+        <v>255</v>
       </c>
       <c r="C40" t="s">
-        <v>134</v>
-      </c>
-      <c r="D40" t="s">
-        <v>135</v>
+        <v>256</v>
+      </c>
+      <c r="E40" t="s">
+        <v>257</v>
       </c>
       <c r="F40" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,5DN,Fifth Dawn,FD,</v>
+        <f>A40&amp;","&amp;B40&amp;","&amp;C40&amp;","&amp;D40&amp;","&amp;E40</f>
+        <v>Special Sets,DDI,Duel Decks: Venser vs. Koth,,Duel Decks - Venser vs. Koth</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>273</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
+        <v>272</v>
       </c>
       <c r="E41" t="s">
-        <v>48</v>
+        <v>272</v>
       </c>
       <c r="F41" t="str">
-        <f t="shared" si="0"/>
-        <v>Core Sets,5E,Fifth Edition,,5th Edition</v>
+        <f>A41&amp;","&amp;B41&amp;","&amp;C41&amp;","&amp;D41&amp;","&amp;E41</f>
+        <v>Special Sets,DDJ,Duel Decks: Izzet vs. Golgari,,Duel Decks: Izzet vs. Golgari</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>29</v>
+        <v>275</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>274</v>
       </c>
       <c r="E42" t="s">
-        <v>31</v>
+        <v>274</v>
       </c>
       <c r="F42" t="str">
-        <f t="shared" si="0"/>
-        <v>Core Sets,4E,Fourth Edition,,4th Edition</v>
+        <f>A42&amp;","&amp;B42&amp;","&amp;C42&amp;","&amp;D42&amp;","&amp;E42</f>
+        <v>Special Sets,DDK,Duel Decks: Sorin vs. Tibalt,,Duel Decks: Sorin vs. Tibalt</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2055,89 +2091,77 @@
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>180</v>
+        <v>271</v>
       </c>
       <c r="C43" t="s">
-        <v>181</v>
+        <v>270</v>
       </c>
       <c r="E43" t="s">
-        <v>182</v>
+        <v>270</v>
       </c>
       <c r="F43" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,DRB,From the Vault: Dragons,,From the Vault - Dragons</v>
+        <f>A43&amp;","&amp;B43&amp;","&amp;C43&amp;","&amp;D43&amp;","&amp;E43</f>
+        <v>Special Sets,DDL,Duel Decks: Heroes vs. Monsters,,Duel Decks: Heroes vs. Monsters</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>198</v>
+        <v>269</v>
       </c>
       <c r="C44" t="s">
-        <v>199</v>
-      </c>
-      <c r="E44" t="s">
-        <v>200</v>
+        <v>268</v>
       </c>
       <c r="F44" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,V09,From the Vault: Exiled,,From the Vault - Exiled</v>
+        <f>A44&amp;","&amp;B44&amp;","&amp;C44&amp;","&amp;D44&amp;","&amp;E44</f>
+        <v>Expansions,DGM,Dragon's Maze,,</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>242</v>
+        <v>153</v>
       </c>
       <c r="C45" t="s">
-        <v>243</v>
-      </c>
-      <c r="E45" t="s">
-        <v>244</v>
+        <v>154</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,V11,From the Vault: Legends,,From the Vault - Legends</v>
+        <f>A45&amp;","&amp;B45&amp;","&amp;C45&amp;","&amp;D45&amp;","&amp;E45</f>
+        <v>Expansions,DIS,Dissension,,</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>277</v>
+        <v>25</v>
       </c>
       <c r="C46" t="s">
-        <v>276</v>
-      </c>
-      <c r="E46" t="s">
-        <v>276</v>
+        <v>26</v>
       </c>
       <c r="F46" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,V12,From the Vault: Realms,,From the Vault: Realms</v>
+        <f>A46&amp;","&amp;B46&amp;","&amp;C46&amp;","&amp;D46&amp;","&amp;E46</f>
+        <v>Expansions,DK,The Dark,,</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
       <c r="C47" t="s">
-        <v>223</v>
-      </c>
-      <c r="E47" t="s">
-        <v>224</v>
+        <v>254</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,V10,From the Vault: Relics,,From the Vault - Relics</v>
+        <f>A47&amp;","&amp;B47&amp;","&amp;C47&amp;","&amp;D47&amp;","&amp;E47</f>
+        <v>Expansions,DKA,Dark Ascension,,</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2145,17 +2169,17 @@
         <v>34</v>
       </c>
       <c r="B48" t="s">
-        <v>279</v>
+        <v>180</v>
       </c>
       <c r="C48" t="s">
-        <v>278</v>
+        <v>181</v>
       </c>
       <c r="E48" t="s">
-        <v>278</v>
+        <v>182</v>
       </c>
       <c r="F48" t="str">
-        <f t="shared" si="0"/>
-        <v>Special Sets,V13,From the Vault: Twenty,,From the Vault: Twenty</v>
+        <f>A48&amp;","&amp;B48&amp;","&amp;C48&amp;","&amp;D48&amp;","&amp;E48</f>
+        <v>Special Sets,DRB,From the Vault: Dragons,,From the Vault - Dragons</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2163,14 +2187,17 @@
         <v>13</v>
       </c>
       <c r="B49" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
       <c r="C49" t="s">
-        <v>165</v>
+        <v>131</v>
+      </c>
+      <c r="D49" t="s">
+        <v>132</v>
       </c>
       <c r="F49" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,FUT,Future Sight,,</v>
+        <f>A49&amp;","&amp;B49&amp;","&amp;C49&amp;","&amp;D49&amp;","&amp;E49</f>
+        <v>Expansions,DST,Darksteel,DS,</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2178,32 +2205,32 @@
         <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>281</v>
+        <v>178</v>
       </c>
       <c r="C50" t="s">
-        <v>280</v>
+        <v>179</v>
       </c>
       <c r="F50" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,GTC,Gatecrash,,</v>
+        <f>A50&amp;","&amp;B50&amp;","&amp;C50&amp;","&amp;D50&amp;","&amp;E50</f>
+        <v>Expansions,EVE,Eventide,,</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B51" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="C51" t="s">
-        <v>151</v>
-      </c>
-      <c r="D51" t="s">
-        <v>152</v>
+        <v>172</v>
+      </c>
+      <c r="E51" t="s">
+        <v>173</v>
       </c>
       <c r="F51" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,GPT,Guildpact,GP,</v>
+        <f>A51&amp;","&amp;B51&amp;","&amp;C51&amp;","&amp;D51&amp;","&amp;E51</f>
+        <v>Special Sets,EVG,Duel Decks: Elves vs. Goblins,,Duel Decks - Elves vs. Goblins</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2211,17 +2238,14 @@
         <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C52" t="s">
-        <v>38</v>
-      </c>
-      <c r="D52" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,HM,Homelands,HL,</v>
+        <f>A52&amp;","&amp;B52&amp;","&amp;C52&amp;","&amp;D52&amp;","&amp;E52</f>
+        <v>Expansions,EX,Exodus,,</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2229,14 +2253,14 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C53" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F53" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,IA,Ice Age,,</v>
+        <f>A53&amp;","&amp;B53&amp;","&amp;C53&amp;","&amp;D53&amp;","&amp;E53</f>
+        <v>Expansions,FE,Fallen Empires,,</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2244,14 +2268,14 @@
         <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>248</v>
+        <v>164</v>
       </c>
       <c r="C54" t="s">
-        <v>249</v>
+        <v>165</v>
       </c>
       <c r="F54" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,ISD,Innistrad,,</v>
+        <f>A54&amp;","&amp;B54&amp;","&amp;C54&amp;","&amp;D54&amp;","&amp;E54</f>
+        <v>Expansions,FUT,Future Sight,,</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2259,14 +2283,17 @@
         <v>13</v>
       </c>
       <c r="B55" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="C55" t="s">
-        <v>96</v>
+        <v>151</v>
+      </c>
+      <c r="D55" t="s">
+        <v>152</v>
       </c>
       <c r="F55" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,IN,Invasion,,</v>
+        <f>A55&amp;","&amp;B55&amp;","&amp;C55&amp;","&amp;D55&amp;","&amp;E55</f>
+        <v>Expansions,GPT,Guildpact,GP,</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2274,17 +2301,14 @@
         <v>13</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>281</v>
       </c>
       <c r="C56" t="s">
-        <v>113</v>
-      </c>
-      <c r="D56" t="s">
-        <v>114</v>
+        <v>280</v>
       </c>
       <c r="F56" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,JUD,Judgment,JU,</v>
+        <f>A56&amp;","&amp;B56&amp;","&amp;C56&amp;","&amp;D56&amp;","&amp;E56</f>
+        <v>Expansions,GTC,Gatecrash,,</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2292,77 +2316,68 @@
         <v>13</v>
       </c>
       <c r="B57" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C57" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="D57" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="F57" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,LE,Legends,LG,</v>
+        <f>A57&amp;","&amp;B57&amp;","&amp;C57&amp;","&amp;D57&amp;","&amp;E57</f>
+        <v>Expansions,GU,Urza's Legacy,UL,</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B58" t="s">
-        <v>118</v>
+        <v>208</v>
       </c>
       <c r="C58" t="s">
-        <v>119</v>
-      </c>
-      <c r="D58" t="s">
-        <v>22</v>
+        <v>209</v>
+      </c>
+      <c r="E58" t="s">
+        <v>210</v>
       </c>
       <c r="F58" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,LGN,Legions,LE,</v>
+        <f>A58&amp;","&amp;B58&amp;","&amp;C58&amp;","&amp;D58&amp;","&amp;E58</f>
+        <v>Special Sets,H09,Premium Deck Series: Slivers,,Premium Deck Series - Slivers</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B59" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="C59" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="D59" t="s">
-        <v>3</v>
-      </c>
-      <c r="E59" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="F59" t="str">
-        <f t="shared" si="0"/>
-        <v>Core Sets,1E,Limited Edition Alpha,A,1st Limited Edition Alpha</v>
+        <f>A59&amp;","&amp;B59&amp;","&amp;C59&amp;","&amp;D59&amp;","&amp;E59</f>
+        <v>Expansions,HM,Homelands,HL,</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>201</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" t="s">
-        <v>7</v>
-      </c>
-      <c r="E60" t="s">
-        <v>8</v>
+        <v>202</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" si="0"/>
-        <v>Core Sets,2E,Limited Edition Beta,B,1st Limited Edition Beta</v>
+        <f>A60&amp;","&amp;B60&amp;","&amp;C60&amp;","&amp;D60&amp;","&amp;E60</f>
+        <v>Special Sets,HOP,Planechase,,</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2370,89 +2385,98 @@
         <v>13</v>
       </c>
       <c r="B61" t="s">
-        <v>169</v>
+        <v>32</v>
       </c>
       <c r="C61" t="s">
-        <v>170</v>
+        <v>33</v>
       </c>
       <c r="F61" t="str">
-        <f t="shared" si="0"/>
-        <v>Expansions,LRW,Lorwyn,,</v>
+        <f>A61&amp;","&amp;B61&amp;","&amp;C61&amp;","&amp;D61&amp;","&amp;E61</f>
+        <v>Expansions,IA,Ice Age,,</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B62" t="s">
-        <v>196</v>
+        <v>95</v>
       </c>
       <c r="C62" t="s">
-        <v>197</v>
+        <v>96</v>
       </c>
       <c r="F62" t="str">
-        <f t="shared" si="0"/>
-        <v>Core Sets,M10,Magic 2010,,</v>
+        <f>A62&amp;","&amp;B62&amp;","&amp;C62&amp;","&amp;D62&amp;","&amp;E62</f>
+        <v>Expansions,IN,Invasion,,</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B63" t="s">
-        <v>220</v>
+        <v>248</v>
       </c>
       <c r="C63" t="s">
-        <v>221</v>
+        <v>249</v>
       </c>
       <c r="F63" t="str">
-        <f t="shared" si="0"/>
-        <v>Core Sets,M11,Magic 2011,,</v>
+        <f>A63&amp;","&amp;B63&amp;","&amp;C63&amp;","&amp;D63&amp;","&amp;E63</f>
+        <v>Expansions,ISD,Innistrad,,</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B64" t="s">
-        <v>240</v>
+        <v>112</v>
       </c>
       <c r="C64" t="s">
-        <v>241</v>
+        <v>113</v>
+      </c>
+      <c r="D64" t="s">
+        <v>114</v>
       </c>
       <c r="F64" t="str">
-        <f t="shared" si="0"/>
-        <v>Core Sets,M12,Magic 2012,,</v>
+        <f>A64&amp;","&amp;B64&amp;","&amp;C64&amp;","&amp;D64&amp;","&amp;E64</f>
+        <v>Expansions,JUD,Judgment,JU,</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B65" t="s">
-        <v>283</v>
+        <v>22</v>
       </c>
       <c r="C65" t="s">
-        <v>282</v>
+        <v>23</v>
+      </c>
+      <c r="D65" t="s">
+        <v>24</v>
       </c>
       <c r="F65" t="str">
-        <f t="shared" si="0"/>
-        <v>Core Sets,M13,Magic 2013,,</v>
+        <f>A65&amp;","&amp;B65&amp;","&amp;C65&amp;","&amp;D65&amp;","&amp;E65</f>
+        <v>Expansions,LE,Legends,LG,</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B66" t="s">
-        <v>285</v>
+        <v>118</v>
       </c>
       <c r="C66" t="s">
-        <v>284</v>
+        <v>119</v>
+      </c>
+      <c r="D66" t="s">
+        <v>22</v>
       </c>
       <c r="F66" t="str">
-        <f t="shared" ref="F66:F122" si="1">A66&amp;","&amp;B66&amp;","&amp;C66&amp;","&amp;D66&amp;","&amp;E66</f>
-        <v>Core Sets,M14,Magic 2014,,</v>
+        <f>A66&amp;","&amp;B66&amp;","&amp;C66&amp;","&amp;D66&amp;","&amp;E66</f>
+        <v>Expansions,LGN,Legions,LE,</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2460,92 +2484,89 @@
         <v>13</v>
       </c>
       <c r="B67" t="s">
-        <v>81</v>
+        <v>169</v>
       </c>
       <c r="C67" t="s">
-        <v>82</v>
+        <v>170</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,MM,Mercadian Masques,,</v>
+        <f>A67&amp;","&amp;B67&amp;","&amp;C67&amp;","&amp;D67&amp;","&amp;E67</f>
+        <v>Expansions,LRW,Lorwyn,,</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B68" t="s">
-        <v>42</v>
+        <v>196</v>
       </c>
       <c r="C68" t="s">
-        <v>43</v>
+        <v>197</v>
       </c>
       <c r="F68" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,MI,Mirage,,</v>
+        <f>A68&amp;","&amp;B68&amp;","&amp;C68&amp;","&amp;D68&amp;","&amp;E68</f>
+        <v>Core Sets,M10,Magic 2010,,</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B69" t="s">
-        <v>127</v>
+        <v>220</v>
       </c>
       <c r="C69" t="s">
-        <v>128</v>
-      </c>
-      <c r="D69" t="s">
-        <v>129</v>
+        <v>221</v>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,MRD,Mirrodin,MR,</v>
+        <f>A69&amp;","&amp;B69&amp;","&amp;C69&amp;","&amp;D69&amp;","&amp;E69</f>
+        <v>Core Sets,M11,Magic 2011,,</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B70" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="C70" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,MBS,Mirrodin Besieged,,</v>
+        <f>A70&amp;","&amp;B70&amp;","&amp;C70&amp;","&amp;D70&amp;","&amp;E70</f>
+        <v>Core Sets,M12,Magic 2012,,</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C71" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F71" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,MMA,Modern Masters,,</v>
+        <f>A71&amp;","&amp;B71&amp;","&amp;C71&amp;","&amp;D71&amp;","&amp;E71</f>
+        <v>Core Sets,M13,Magic 2013,,</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>174</v>
+        <v>285</v>
       </c>
       <c r="C72" t="s">
-        <v>175</v>
+        <v>284</v>
       </c>
       <c r="F72" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,MOR,Morningtide,,</v>
+        <f>A72&amp;","&amp;B72&amp;","&amp;C72&amp;","&amp;D72&amp;","&amp;E72</f>
+        <v>Core Sets,M14,Magic 2014,,</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2553,83 +2574,74 @@
         <v>13</v>
       </c>
       <c r="B73" t="s">
-        <v>87</v>
+        <v>233</v>
       </c>
       <c r="C73" t="s">
-        <v>88</v>
+        <v>234</v>
       </c>
       <c r="F73" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,NE,Nemesis,,</v>
+        <f>A73&amp;","&amp;B73&amp;","&amp;C73&amp;","&amp;D73&amp;","&amp;E73</f>
+        <v>Expansions,MBS,Mirrodin Besieged,,</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B74" t="s">
-        <v>238</v>
+        <v>295</v>
       </c>
       <c r="C74" t="s">
-        <v>239</v>
+        <v>299</v>
       </c>
       <c r="F74" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,NPH,New Phyrexia,,</v>
+        <f>A74&amp;","&amp;B74&amp;","&amp;C74&amp;","&amp;D74&amp;","&amp;E74</f>
+        <v>Special Sets,ME2,Master's Edition II,,</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B75" t="s">
-        <v>144</v>
+        <v>296</v>
       </c>
       <c r="C75" t="s">
-        <v>145</v>
-      </c>
-      <c r="D75" t="s">
-        <v>146</v>
-      </c>
-      <c r="E75" t="s">
-        <v>147</v>
+        <v>300</v>
       </c>
       <c r="F75" t="str">
-        <f t="shared" si="1"/>
-        <v>Core Sets,9ED,Ninth Edition,9E,9th Edition</v>
+        <f>A75&amp;","&amp;B75&amp;","&amp;C75&amp;","&amp;D75&amp;","&amp;E75</f>
+        <v>Special Sets,ME3,Master's Edition III,,</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B76" t="s">
-        <v>107</v>
+        <v>297</v>
       </c>
       <c r="C76" t="s">
-        <v>108</v>
+        <v>301</v>
       </c>
       <c r="F76" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,OD,Odyssey,,</v>
+        <f>A76&amp;","&amp;B76&amp;","&amp;C76&amp;","&amp;D76&amp;","&amp;E76</f>
+        <v>Special Sets,ME4,Master's Edition IV,,</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B77" t="s">
-        <v>115</v>
+        <v>298</v>
       </c>
       <c r="C77" t="s">
-        <v>116</v>
-      </c>
-      <c r="D77" t="s">
-        <v>117</v>
+        <v>294</v>
       </c>
       <c r="F77" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,ONS,Onslaught,ON,</v>
+        <f>A77&amp;","&amp;B77&amp;","&amp;C77&amp;","&amp;D77&amp;","&amp;E77</f>
+        <v>Special Sets,MED,Master's Edition,,</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2637,29 +2649,29 @@
         <v>13</v>
       </c>
       <c r="B78" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
       <c r="C78" t="s">
-        <v>163</v>
+        <v>43</v>
       </c>
       <c r="F78" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,PLC,Planar Chaos,,</v>
+        <f>A78&amp;","&amp;B78&amp;","&amp;C78&amp;","&amp;D78&amp;","&amp;E78</f>
+        <v>Expansions,MI,Mirage,,</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B79" t="s">
-        <v>201</v>
+        <v>81</v>
       </c>
       <c r="C79" t="s">
-        <v>202</v>
+        <v>82</v>
       </c>
       <c r="F79" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,HOP,Planechase,,</v>
+        <f>A79&amp;","&amp;B79&amp;","&amp;C79&amp;","&amp;D79&amp;","&amp;E79</f>
+        <v>Expansions,MM,Mercadian Masques,,</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2667,14 +2679,14 @@
         <v>34</v>
       </c>
       <c r="B80" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C80" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F80" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,PC2,Planechase (2012 Edition),,</v>
+        <f>A80&amp;","&amp;B80&amp;","&amp;C80&amp;","&amp;D80&amp;","&amp;E80</f>
+        <v>Special Sets,MMA,Modern Masters,,</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2682,101 +2694,95 @@
         <v>13</v>
       </c>
       <c r="B81" t="s">
-        <v>100</v>
+        <v>174</v>
       </c>
       <c r="C81" t="s">
-        <v>101</v>
+        <v>175</v>
       </c>
       <c r="F81" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,PS,Planeshift,,</v>
+        <f>A81&amp;","&amp;B81&amp;","&amp;C81&amp;","&amp;D81&amp;","&amp;E81</f>
+        <v>Expansions,MOR,Morningtide,,</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B82" t="s">
-        <v>49</v>
+        <v>127</v>
       </c>
       <c r="C82" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="D82" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="F82" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,PO,Portal,PT,</v>
+        <f>A82&amp;","&amp;B82&amp;","&amp;C82&amp;","&amp;D82&amp;","&amp;E82</f>
+        <v>Expansions,MRD,Mirrodin,MR,</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B83" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="C83" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="F83" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,P2,Portal Second Age,,</v>
+        <f>A83&amp;","&amp;B83&amp;","&amp;C83&amp;","&amp;D83&amp;","&amp;E83</f>
+        <v>Expansions,NE,Nemesis,,</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B84" t="s">
-        <v>77</v>
+        <v>238</v>
       </c>
       <c r="C84" t="s">
-        <v>78</v>
-      </c>
-      <c r="D84" t="s">
-        <v>79</v>
+        <v>239</v>
       </c>
       <c r="F84" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,PK,Portal Three Kingdoms,P3,</v>
+        <f>A84&amp;","&amp;B84&amp;","&amp;C84&amp;","&amp;D84&amp;","&amp;E84</f>
+        <v>Expansions,NPH,New Phyrexia,,</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B85" t="s">
-        <v>230</v>
+        <v>107</v>
       </c>
       <c r="C85" t="s">
-        <v>231</v>
-      </c>
-      <c r="E85" t="s">
-        <v>232</v>
+        <v>108</v>
       </c>
       <c r="F85" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,PD2,Premium Deck Series: Fire and Lightning,,Premium Deck Series - Fire &amp; Lightning</v>
+        <f>A85&amp;","&amp;B85&amp;","&amp;C85&amp;","&amp;D85&amp;","&amp;E85</f>
+        <v>Expansions,OD,Odyssey,,</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B86" t="s">
-        <v>250</v>
+        <v>115</v>
       </c>
       <c r="C86" t="s">
-        <v>251</v>
-      </c>
-      <c r="E86" t="s">
-        <v>252</v>
+        <v>116</v>
+      </c>
+      <c r="D86" t="s">
+        <v>117</v>
       </c>
       <c r="F86" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,PD3,Premium Deck Series: Graveborn,,Premium Deck Series - Graveborn</v>
+        <f>A86&amp;","&amp;B86&amp;","&amp;C86&amp;","&amp;D86&amp;","&amp;E86</f>
+        <v>Expansions,ONS,Onslaught,ON,</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2784,116 +2790,119 @@
         <v>34</v>
       </c>
       <c r="B87" t="s">
-        <v>208</v>
+        <v>61</v>
       </c>
       <c r="C87" t="s">
-        <v>209</v>
-      </c>
-      <c r="E87" t="s">
-        <v>210</v>
+        <v>62</v>
       </c>
       <c r="F87" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,H09,Premium Deck Series: Slivers,,Premium Deck Series - Slivers</v>
+        <f>A87&amp;","&amp;B87&amp;","&amp;C87&amp;","&amp;D87&amp;","&amp;E87</f>
+        <v>Special Sets,P2,Portal Second Age,,</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B88" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C88" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D88" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="F88" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,PR,Prophecy,PY,</v>
+        <f>A88&amp;","&amp;B88&amp;","&amp;C88&amp;","&amp;D88&amp;","&amp;E88</f>
+        <v>Special Sets,P3,Starter 1999,ST,</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B89" t="s">
-        <v>148</v>
+        <v>89</v>
       </c>
       <c r="C89" t="s">
-        <v>149</v>
+        <v>90</v>
+      </c>
+      <c r="D89" t="s">
+        <v>91</v>
       </c>
       <c r="F89" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,RAV,Ravnica: City of Guilds,,</v>
+        <f>A89&amp;","&amp;B89&amp;","&amp;C89&amp;","&amp;D89&amp;","&amp;E89</f>
+        <v>Special Sets,P4,Starter 2000,S00,</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B90" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C90" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F90" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,RTR,Return to Ravnica,,</v>
+        <f>A90&amp;","&amp;B90&amp;","&amp;C90&amp;","&amp;D90&amp;","&amp;E90</f>
+        <v>Special Sets,PC2,Planechase (2012 Edition),,</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B91" t="s">
-        <v>18</v>
+        <v>230</v>
       </c>
       <c r="C91" t="s">
-        <v>19</v>
-      </c>
-      <c r="D91" t="s">
-        <v>20</v>
+        <v>231</v>
       </c>
       <c r="E91" t="s">
-        <v>21</v>
+        <v>232</v>
       </c>
       <c r="F91" t="str">
-        <f t="shared" si="1"/>
-        <v>Core Sets,3E,Revised Edition,R,3rd Revised Edition</v>
+        <f>A91&amp;","&amp;B91&amp;","&amp;C91&amp;","&amp;D91&amp;","&amp;E91</f>
+        <v>Special Sets,PD2,Premium Deck Series: Fire and Lightning,,Premium Deck Series - Fire &amp; Lightning</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B92" t="s">
-        <v>216</v>
+        <v>250</v>
       </c>
       <c r="C92" t="s">
-        <v>217</v>
+        <v>251</v>
+      </c>
+      <c r="E92" t="s">
+        <v>252</v>
       </c>
       <c r="F92" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,ROE,Rise of the Eldrazi,,</v>
+        <f>A92&amp;","&amp;B92&amp;","&amp;C92&amp;","&amp;D92&amp;","&amp;E92</f>
+        <v>Special Sets,PD3,Premium Deck Series: Graveborn,,Premium Deck Series - Graveborn</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B93" t="s">
-        <v>142</v>
+        <v>77</v>
       </c>
       <c r="C93" t="s">
-        <v>143</v>
+        <v>78</v>
+      </c>
+      <c r="D93" t="s">
+        <v>79</v>
       </c>
       <c r="F93" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,SOK,Saviors of Kamigawa,,</v>
+        <f>A93&amp;","&amp;B93&amp;","&amp;C93&amp;","&amp;D93&amp;","&amp;E93</f>
+        <v>Special Sets,PK,Portal Three Kingdoms,P3,</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2901,50 +2910,50 @@
         <v>13</v>
       </c>
       <c r="B94" t="s">
-        <v>228</v>
+        <v>162</v>
       </c>
       <c r="C94" t="s">
-        <v>229</v>
+        <v>163</v>
       </c>
       <c r="F94" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,SOM,Scars of Mirrodin,,</v>
+        <f>A94&amp;","&amp;B94&amp;","&amp;C94&amp;","&amp;D94&amp;","&amp;E94</f>
+        <v>Expansions,PLC,Planar Chaos,,</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B95" t="s">
-        <v>120</v>
+        <v>49</v>
       </c>
       <c r="C95" t="s">
-        <v>121</v>
+        <v>50</v>
       </c>
       <c r="D95" t="s">
-        <v>122</v>
+        <v>51</v>
       </c>
       <c r="F95" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,SCG,Scourge,SC,</v>
+        <f>A95&amp;","&amp;B95&amp;","&amp;C95&amp;","&amp;D95&amp;","&amp;E95</f>
+        <v>Special Sets,PO,Portal,PT,</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B96" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C96" t="s">
-        <v>103</v>
-      </c>
-      <c r="E96" t="s">
-        <v>104</v>
+        <v>93</v>
+      </c>
+      <c r="D96" t="s">
+        <v>94</v>
       </c>
       <c r="F96" t="str">
-        <f t="shared" si="1"/>
-        <v>Core Sets,7E,Seventh Edition,,7th Edition</v>
+        <f>A96&amp;","&amp;B96&amp;","&amp;C96&amp;","&amp;D96&amp;","&amp;E96</f>
+        <v>Expansions,PR,Prophecy,PY,</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2952,14 +2961,14 @@
         <v>13</v>
       </c>
       <c r="B97" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="C97" t="s">
-        <v>177</v>
+        <v>101</v>
       </c>
       <c r="F97" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,SHM,Shadowmoor,,</v>
+        <f>A97&amp;","&amp;B97&amp;","&amp;C97&amp;","&amp;D97&amp;","&amp;E97</f>
+        <v>Expansions,PS,Planeshift,,</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2967,50 +2976,44 @@
         <v>13</v>
       </c>
       <c r="B98" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
       <c r="C98" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="F98" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,ALA,Shards of Alara,,</v>
+        <f>A98&amp;","&amp;B98&amp;","&amp;C98&amp;","&amp;D98&amp;","&amp;E98</f>
+        <v>Expansions,RAV,Ravnica: City of Guilds,,</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B99" t="s">
-        <v>79</v>
+        <v>216</v>
       </c>
       <c r="C99" t="s">
-        <v>80</v>
-      </c>
-      <c r="D99" t="s">
-        <v>56</v>
+        <v>217</v>
       </c>
       <c r="F99" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,P3,Starter 1999,ST,</v>
+        <f>A99&amp;","&amp;B99&amp;","&amp;C99&amp;","&amp;D99&amp;","&amp;E99</f>
+        <v>Expansions,ROE,Rise of the Eldrazi,,</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B100" t="s">
-        <v>89</v>
+        <v>291</v>
       </c>
       <c r="C100" t="s">
-        <v>90</v>
-      </c>
-      <c r="D100" t="s">
-        <v>91</v>
+        <v>290</v>
       </c>
       <c r="F100" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,P4,Starter 2000,S00,</v>
+        <f>A100&amp;","&amp;B100&amp;","&amp;C100&amp;","&amp;D100&amp;","&amp;E100</f>
+        <v>Expansions,RTR,Return to Ravnica,,</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -3018,17 +3021,17 @@
         <v>13</v>
       </c>
       <c r="B101" t="s">
-        <v>56</v>
+        <v>120</v>
       </c>
       <c r="C101" t="s">
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="D101" t="s">
-        <v>58</v>
+        <v>122</v>
       </c>
       <c r="F101" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,ST,Stronghold,SH,</v>
+        <f>A101&amp;","&amp;B101&amp;","&amp;C101&amp;","&amp;D101&amp;","&amp;E101</f>
+        <v>Expansions,SCG,Scourge,SC,</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -3036,32 +3039,29 @@
         <v>13</v>
       </c>
       <c r="B102" t="s">
-        <v>54</v>
+        <v>176</v>
       </c>
       <c r="C102" t="s">
-        <v>55</v>
+        <v>177</v>
       </c>
       <c r="F102" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,TE,Tempest,,</v>
+        <f>A102&amp;","&amp;B102&amp;","&amp;C102&amp;","&amp;D102&amp;","&amp;E102</f>
+        <v>Expansions,SHM,Shadowmoor,,</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B103" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="C103" t="s">
-        <v>167</v>
-      </c>
-      <c r="E103" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="F103" t="str">
-        <f t="shared" si="1"/>
-        <v>Core Sets,10E,Tenth Edition,,10th Edition</v>
+        <f>A103&amp;","&amp;B103&amp;","&amp;C103&amp;","&amp;D103&amp;","&amp;E103</f>
+        <v>Expansions,SOK,Saviors of Kamigawa,,</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -3069,14 +3069,14 @@
         <v>13</v>
       </c>
       <c r="B104" t="s">
-        <v>25</v>
+        <v>228</v>
       </c>
       <c r="C104" t="s">
-        <v>26</v>
+        <v>229</v>
       </c>
       <c r="F104" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,DK,The Dark,,</v>
+        <f>A104&amp;","&amp;B104&amp;","&amp;C104&amp;","&amp;D104&amp;","&amp;E104</f>
+        <v>Expansions,SOM,Scars of Mirrodin,,</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -3084,14 +3084,17 @@
         <v>13</v>
       </c>
       <c r="B105" t="s">
-        <v>293</v>
+        <v>56</v>
       </c>
       <c r="C105" t="s">
-        <v>292</v>
+        <v>57</v>
+      </c>
+      <c r="D105" t="s">
+        <v>58</v>
       </c>
       <c r="F105" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,THS,Theros,,</v>
+        <f>A105&amp;","&amp;B105&amp;","&amp;C105&amp;","&amp;D105&amp;","&amp;E105</f>
+        <v>Expansions,ST,Stronghold,SH,</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -3099,14 +3102,14 @@
         <v>13</v>
       </c>
       <c r="B106" t="s">
-        <v>158</v>
+        <v>54</v>
       </c>
       <c r="C106" t="s">
-        <v>159</v>
+        <v>55</v>
       </c>
       <c r="F106" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,TSP,Time Spiral,,</v>
+        <f>A106&amp;","&amp;B106&amp;","&amp;C106&amp;","&amp;D106&amp;","&amp;E106</f>
+        <v>Expansions,TE,Tempest,,</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -3114,14 +3117,14 @@
         <v>13</v>
       </c>
       <c r="B107" t="s">
-        <v>160</v>
+        <v>293</v>
       </c>
       <c r="C107" t="s">
-        <v>161</v>
+        <v>292</v>
       </c>
       <c r="F107" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,TSB,Time Spiral "Timeshifted",,</v>
+        <f>A107&amp;","&amp;B107&amp;","&amp;C107&amp;","&amp;D107&amp;","&amp;E107</f>
+        <v>Expansions,THS,Theros,,</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -3138,77 +3141,68 @@
         <v>111</v>
       </c>
       <c r="F108" t="str">
-        <f t="shared" si="1"/>
+        <f>A108&amp;","&amp;B108&amp;","&amp;C108&amp;","&amp;D108&amp;","&amp;E108</f>
         <v>Expansions,TOR,Torment,TO,</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B109" t="s">
-        <v>63</v>
+        <v>160</v>
       </c>
       <c r="C109" t="s">
-        <v>64</v>
+        <v>161</v>
       </c>
       <c r="F109" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,UG,Unglued,,</v>
+        <f>A109&amp;","&amp;B109&amp;","&amp;C109&amp;","&amp;D109&amp;","&amp;E109</f>
+        <v>Expansions,TSB,Time Spiral "Timeshifted",,</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B110" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="C110" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="F110" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,UNH,Unhinged,,</v>
+        <f>A110&amp;","&amp;B110&amp;","&amp;C110&amp;","&amp;D110&amp;","&amp;E110</f>
+        <v>Expansions,TSP,Time Spiral,,</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B111" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="C111" t="s">
-        <v>10</v>
-      </c>
-      <c r="D111" t="s">
-        <v>11</v>
-      </c>
-      <c r="E111" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="F111" t="str">
-        <f t="shared" si="1"/>
-        <v>Core Sets,2U,Unlimited Edition,U,2nd Unlimited</v>
+        <f>A111&amp;","&amp;B111&amp;","&amp;C111&amp;","&amp;D111&amp;","&amp;E111</f>
+        <v>Special Sets,UG,Unglued,,</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B112" t="s">
-        <v>74</v>
+        <v>138</v>
       </c>
       <c r="C112" t="s">
-        <v>75</v>
-      </c>
-      <c r="D112" t="s">
-        <v>76</v>
+        <v>139</v>
       </c>
       <c r="F112" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,CG,Urza's Destiny,UD,</v>
+        <f>A112&amp;","&amp;B112&amp;","&amp;C112&amp;","&amp;D112&amp;","&amp;E112</f>
+        <v>Special Sets,UNH,Unhinged,,</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -3216,159 +3210,193 @@
         <v>13</v>
       </c>
       <c r="B113" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C113" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D113" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F113" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,GU,Urza's Legacy,UL,</v>
+        <f>A113&amp;","&amp;B113&amp;","&amp;C113&amp;","&amp;D113&amp;","&amp;E113</f>
+        <v>Expansions,UZ,Urza's Saga,US,</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B114" t="s">
-        <v>65</v>
+        <v>198</v>
       </c>
       <c r="C114" t="s">
-        <v>66</v>
-      </c>
-      <c r="D114" t="s">
-        <v>67</v>
+        <v>199</v>
+      </c>
+      <c r="E114" t="s">
+        <v>200</v>
       </c>
       <c r="F114" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,UZ,Urza's Saga,US,</v>
+        <f>A114&amp;","&amp;B114&amp;","&amp;C114&amp;","&amp;D114&amp;","&amp;E114</f>
+        <v>Special Sets,V09,From the Vault: Exiled,,From the Vault - Exiled</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B115" t="s">
-        <v>44</v>
+        <v>222</v>
       </c>
       <c r="C115" t="s">
-        <v>45</v>
+        <v>223</v>
+      </c>
+      <c r="E115" t="s">
+        <v>224</v>
       </c>
       <c r="F115" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,VI,Visions,,</v>
+        <f>A115&amp;","&amp;B115&amp;","&amp;C115&amp;","&amp;D115&amp;","&amp;E115</f>
+        <v>Special Sets,V10,From the Vault: Relics,,From the Vault - Relics</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B116" t="s">
-        <v>52</v>
+        <v>242</v>
       </c>
       <c r="C116" t="s">
-        <v>53</v>
+        <v>243</v>
+      </c>
+      <c r="E116" t="s">
+        <v>244</v>
       </c>
       <c r="F116" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,WL,Weatherlight,,</v>
+        <f>A116&amp;","&amp;B116&amp;","&amp;C116&amp;","&amp;D116&amp;","&amp;E116</f>
+        <v>Special Sets,V11,From the Vault: Legends,,From the Vault - Legends</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B117" t="s">
-        <v>211</v>
+        <v>277</v>
       </c>
       <c r="C117" t="s">
-        <v>212</v>
+        <v>276</v>
+      </c>
+      <c r="E117" t="s">
+        <v>276</v>
       </c>
       <c r="F117" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,WWK,Worldwake,,</v>
+        <f>A117&amp;","&amp;B117&amp;","&amp;C117&amp;","&amp;D117&amp;","&amp;E117</f>
+        <v>Special Sets,V12,From the Vault: Realms,,From the Vault: Realms</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B118" t="s">
-        <v>203</v>
+        <v>279</v>
       </c>
       <c r="C118" t="s">
-        <v>204</v>
+        <v>278</v>
+      </c>
+      <c r="E118" t="s">
+        <v>278</v>
       </c>
       <c r="F118" t="str">
-        <f t="shared" si="1"/>
-        <v>Expansions,ZEN,Zendikar,,</v>
+        <f>A118&amp;","&amp;B118&amp;","&amp;C118&amp;","&amp;D118&amp;","&amp;E118</f>
+        <v>Special Sets,V13,From the Vault: Twenty,,From the Vault: Twenty</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B119" t="s">
-        <v>298</v>
+        <v>44</v>
       </c>
       <c r="C119" t="s">
-        <v>294</v>
+        <v>45</v>
       </c>
       <c r="F119" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,MED,Master's Edition,,</v>
+        <f>A119&amp;","&amp;B119&amp;","&amp;C119&amp;","&amp;D119&amp;","&amp;E119</f>
+        <v>Expansions,VI,Visions,,</v>
       </c>
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B120" t="s">
-        <v>295</v>
+        <v>52</v>
       </c>
       <c r="C120" t="s">
-        <v>299</v>
+        <v>53</v>
       </c>
       <c r="F120" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,ME2,Master's Edition II,,</v>
+        <f>A120&amp;","&amp;B120&amp;","&amp;C120&amp;","&amp;D120&amp;","&amp;E120</f>
+        <v>Expansions,WL,Weatherlight,,</v>
       </c>
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B121" t="s">
-        <v>296</v>
+        <v>211</v>
       </c>
       <c r="C121" t="s">
-        <v>300</v>
+        <v>212</v>
       </c>
       <c r="F121" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,ME3,Master's Edition III,,</v>
+        <f>A121&amp;","&amp;B121&amp;","&amp;C121&amp;","&amp;D121&amp;","&amp;E121</f>
+        <v>Expansions,WWK,Worldwake,,</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B122" t="s">
-        <v>297</v>
+        <v>203</v>
       </c>
       <c r="C122" t="s">
-        <v>301</v>
+        <v>204</v>
       </c>
       <c r="F122" t="str">
-        <f t="shared" si="1"/>
-        <v>Special Sets,ME4,Master's Edition IV,,</v>
+        <f>A122&amp;","&amp;B122&amp;","&amp;C122&amp;","&amp;D122&amp;","&amp;E122</f>
+        <v>Expansions,ZEN,Zendikar,,</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" t="s">
+        <v>34</v>
+      </c>
+      <c r="B123" t="s">
+        <v>329</v>
+      </c>
+      <c r="C123" t="s">
+        <v>330</v>
+      </c>
+      <c r="E123" t="s">
+        <v>330</v>
+      </c>
+      <c r="F123" t="str">
+        <f>A123&amp;","&amp;B123&amp;","&amp;C123&amp;","&amp;D123&amp;","&amp;E123</f>
+        <v>Special Sets,PPR,Promo set for Gatherer,,Promo set for Gatherer</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:F122">
+    <sortCondition ref="B1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>